<commit_message>
adds day 2 data
</commit_message>
<xml_diff>
--- a/kdt/ex_schedule.xlsx
+++ b/kdt/ex_schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihpar/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihpar/Documents/Deve/bme688/kdt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5457AE0D-0E25-BE45-BAA9-00778049039B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A20B932-D35D-2245-8F0A-C9699C86D76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="7920" windowWidth="33500" windowHeight="17440" xr2:uid="{362ECA0C-1C1C-EB42-A449-6FADEFDCF7ED}"/>
+    <workbookView xWindow="4520" yWindow="10240" windowWidth="33500" windowHeight="17440" xr2:uid="{362ECA0C-1C1C-EB42-A449-6FADEFDCF7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
   <si>
     <t>Dana</t>
   </si>
@@ -100,12 +100,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -183,34 +195,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +601,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="9" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
@@ -562,7 +610,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -570,31 +618,32 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C3" s="3">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13">
         <v>45558</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="1"/>
@@ -603,16 +652,16 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
+      <c r="B6" s="17">
         <v>14.32</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="16">
         <v>1</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="16">
         <v>2</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="16" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="1"/>
@@ -621,95 +670,95 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+      <c r="B7" s="17">
         <v>14.52</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+      <c r="B8" s="17">
         <v>15.02</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="16">
         <v>2</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="B9" s="17">
         <v>15.22</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="B10" s="17">
         <v>15.32</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="16">
         <v>2</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="16">
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="B11" s="17">
         <v>15.52</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+      <c r="B12" s="17">
         <v>16.02</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -717,102 +766,135 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C14" s="3">
+      <c r="B14" s="21"/>
+      <c r="C14" s="22">
         <v>45559</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="B17" s="27">
+        <v>14.3</v>
+      </c>
+      <c r="C17" s="26">
+        <v>1</v>
+      </c>
+      <c r="D17" s="26">
+        <v>2</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="27">
+        <v>14.5</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="27">
+        <v>15</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="26">
+        <v>1</v>
+      </c>
+      <c r="E19" s="26">
+        <v>2</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="27">
+        <v>15.2</v>
+      </c>
+      <c r="C20" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="B21" s="27">
+        <v>15.3</v>
+      </c>
+      <c r="C21" s="26">
+        <v>2</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="26">
+        <v>1</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="27">
+        <v>15.5</v>
+      </c>
+      <c r="C22" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="27">
+        <v>16</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -820,16 +902,16 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C25" s="3">
+      <c r="C25" s="7">
         <v>45560</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -837,85 +919,85 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="5" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="10"/>
+      <c r="C29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="7" t="s">
+      <c r="B31" s="10"/>
+      <c r="C31" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="7" t="s">
+      <c r="B33" s="10"/>
+      <c r="C33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>

</xml_diff>